<commit_message>
update auto send order mt5
</commit_message>
<xml_diff>
--- a/src/pnl_cache/pnl_log.xlsx
+++ b/src/pnl_cache/pnl_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2053"/>
+  <dimension ref="A1:E2108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="91" customWidth="1" min="4" max="4"/>
+    <col width="102" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -43547,6 +43547,1161 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2054">
+      <c r="A2054" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2054" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:00.816137</t>
+        </is>
+      </c>
+      <c r="C2054" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="D2054" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86042, "EURUSDc": 1.1685, "AUDJPYc": 96.646, "EURNZDc": 1.96117, "USDCHFc": 0.80653}</t>
+        </is>
+      </c>
+      <c r="E2054" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2055">
+      <c r="A2055" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2055" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:00.836774</t>
+        </is>
+      </c>
+      <c r="C2055" t="n">
+        <v>37.59</v>
+      </c>
+      <c r="D2055" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59596, "GBPJPYc": 199.88, "EURCADc": 1.60973, "AUDCHFc": 0.52658, "EURUSDc": 1.1685}</t>
+        </is>
+      </c>
+      <c r="E2055" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2056">
+      <c r="A2056" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2056" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:01.834180</t>
+        </is>
+      </c>
+      <c r="C2056" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D2056" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86042, "EURUSDc": 1.1684, "AUDJPYc": 96.649, "EURNZDc": 1.96116, "USDCHFc": 0.80657}</t>
+        </is>
+      </c>
+      <c r="E2056" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2057">
+      <c r="A2057" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2057" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:01.856826</t>
+        </is>
+      </c>
+      <c r="C2057" t="n">
+        <v>37.95</v>
+      </c>
+      <c r="D2057" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.5959, "GBPJPYc": 199.898, "EURCADc": 1.60963, "AUDCHFc": 0.52658, "EURUSDc": 1.1684}</t>
+        </is>
+      </c>
+      <c r="E2057" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2058">
+      <c r="A2058" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2058" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:02.853618</t>
+        </is>
+      </c>
+      <c r="C2058" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="D2058" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86041, "EURUSDc": 1.16839, "AUDJPYc": 96.651, "EURNZDc": 1.96118, "USDCHFc": 0.80658}</t>
+        </is>
+      </c>
+      <c r="E2058" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2059">
+      <c r="A2059" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2059" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:02.869650</t>
+        </is>
+      </c>
+      <c r="C2059" t="n">
+        <v>37.97</v>
+      </c>
+      <c r="D2059" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59591, "GBPJPYc": 199.902, "EURCADc": 1.60963, "AUDCHFc": 0.52657, "EURUSDc": 1.16839}</t>
+        </is>
+      </c>
+      <c r="E2059" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2060">
+      <c r="A2060" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2060" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:03.866576</t>
+        </is>
+      </c>
+      <c r="C2060" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="D2060" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86041, "EURUSDc": 1.16839, "AUDJPYc": 96.651, "EURNZDc": 1.96118, "USDCHFc": 0.80658}</t>
+        </is>
+      </c>
+      <c r="E2060" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2061">
+      <c r="A2061" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2061" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:03.881491</t>
+        </is>
+      </c>
+      <c r="C2061" t="n">
+        <v>37.97</v>
+      </c>
+      <c r="D2061" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59591, "GBPJPYc": 199.902, "EURCADc": 1.60963, "AUDCHFc": 0.52657, "EURUSDc": 1.16839}</t>
+        </is>
+      </c>
+      <c r="E2061" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2062">
+      <c r="A2062" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2062" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:04.891920</t>
+        </is>
+      </c>
+      <c r="C2062" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="D2062" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59592, "GBPJPYc": 199.894, "EURCADc": 1.60963, "AUDCHFc": 0.52658, "EURUSDc": 1.1684}</t>
+        </is>
+      </c>
+      <c r="E2062" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2063">
+      <c r="A2063" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2063" t="inlineStr">
+        <is>
+          <t>2025-08-13T11:07:04.906634</t>
+        </is>
+      </c>
+      <c r="C2063" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="D2063" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.8604, "EURUSDc": 1.1684, "AUDJPYc": 96.652, "EURNZDc": 1.96118, "USDCHFc": 0.80658}</t>
+        </is>
+      </c>
+      <c r="E2063" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2064">
+      <c r="A2064" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2064" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:43.159899</t>
+        </is>
+      </c>
+      <c r="C2064" t="n">
+        <v>-2.57</v>
+      </c>
+      <c r="D2064" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86039, "EURUSDc": 1.16841, "AUDJPYc": 96.65, "EURNZDc": 1.96117, "USDCHFc": 0.80659}</t>
+        </is>
+      </c>
+      <c r="E2064" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2065">
+      <c r="A2065" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2065" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:43.427432</t>
+        </is>
+      </c>
+      <c r="C2065" t="n">
+        <v>31.74</v>
+      </c>
+      <c r="D2065" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59843, "GBPJPYc": 199.695, "EURCADc": 1.61056, "AUDCHFc": 0.52712, "EURUSDc": 1.17078}</t>
+        </is>
+      </c>
+      <c r="E2065" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2066">
+      <c r="A2066" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2066" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:44.179811</t>
+        </is>
+      </c>
+      <c r="C2066" t="n">
+        <v>-2.56</v>
+      </c>
+      <c r="D2066" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86254, "EURUSDc": 1.17078, "AUDJPYc": 96.638, "EURNZDc": 1.95689, "USDCHFc": 0.80455}</t>
+        </is>
+      </c>
+      <c r="E2066" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2067">
+      <c r="A2067" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2067" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:44.442647</t>
+        </is>
+      </c>
+      <c r="C2067" t="n">
+        <v>31.75</v>
+      </c>
+      <c r="D2067" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59843, "GBPJPYc": 199.695, "EURCADc": 1.61055, "AUDCHFc": 0.52712, "EURUSDc": 1.17078}</t>
+        </is>
+      </c>
+      <c r="E2067" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2068">
+      <c r="A2068" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2068" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:45.189132</t>
+        </is>
+      </c>
+      <c r="C2068" t="n">
+        <v>-2.55</v>
+      </c>
+      <c r="D2068" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86254, "EURUSDc": 1.17078, "AUDJPYc": 96.639, "EURNZDc": 1.95689, "USDCHFc": 0.80455}</t>
+        </is>
+      </c>
+      <c r="E2068" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2069">
+      <c r="A2069" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2069" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:45.450449</t>
+        </is>
+      </c>
+      <c r="C2069" t="n">
+        <v>31.68</v>
+      </c>
+      <c r="D2069" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59843, "GBPJPYc": 199.685, "EURCADc": 1.61055, "AUDCHFc": 0.52714, "EURUSDc": 1.17081}</t>
+        </is>
+      </c>
+      <c r="E2069" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2070">
+      <c r="A2070" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2070" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:46.211081</t>
+        </is>
+      </c>
+      <c r="C2070" t="n">
+        <v>-2.56</v>
+      </c>
+      <c r="D2070" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86253, "EURUSDc": 1.17081, "AUDJPYc": 96.639, "EURNZDc": 1.95686, "USDCHFc": 0.80454}</t>
+        </is>
+      </c>
+      <c r="E2070" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2071">
+      <c r="A2071" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2071" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:46.457832</t>
+        </is>
+      </c>
+      <c r="C2071" t="n">
+        <v>31.61</v>
+      </c>
+      <c r="D2071" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59845, "GBPJPYc": 199.681, "EURCADc": 1.61055, "AUDCHFc": 0.52713, "EURUSDc": 1.17081}</t>
+        </is>
+      </c>
+      <c r="E2071" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2072">
+      <c r="A2072" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2072" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:47.237850</t>
+        </is>
+      </c>
+      <c r="C2072" t="n">
+        <v>-2.55</v>
+      </c>
+      <c r="D2072" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86251, "EURUSDc": 1.17081, "AUDJPYc": 96.637, "EURNZDc": 1.95684, "USDCHFc": 0.80454}</t>
+        </is>
+      </c>
+      <c r="E2072" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2073">
+      <c r="A2073" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2073" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:47.470170</t>
+        </is>
+      </c>
+      <c r="C2073" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="D2073" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59845, "GBPJPYc": 199.681, "EURCADc": 1.61056, "AUDCHFc": 0.52713, "EURUSDc": 1.17081}</t>
+        </is>
+      </c>
+      <c r="E2073" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2074">
+      <c r="A2074" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2074" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:48.248292</t>
+        </is>
+      </c>
+      <c r="C2074" t="n">
+        <v>-2.54</v>
+      </c>
+      <c r="D2074" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86251, "EURUSDc": 1.17079, "AUDJPYc": 96.637, "EURNZDc": 1.95685, "USDCHFc": 0.80454}</t>
+        </is>
+      </c>
+      <c r="E2074" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2075">
+      <c r="A2075" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2075" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:48.479073</t>
+        </is>
+      </c>
+      <c r="C2075" t="n">
+        <v>31.68</v>
+      </c>
+      <c r="D2075" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59845, "GBPJPYc": 199.688, "EURCADc": 1.61055, "AUDCHFc": 0.52713, "EURUSDc": 1.17079}</t>
+        </is>
+      </c>
+      <c r="E2075" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2076">
+      <c r="A2076" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2076" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:29:49.274161</t>
+        </is>
+      </c>
+      <c r="C2076" t="n">
+        <v>-2.54</v>
+      </c>
+      <c r="D2076" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86252, "EURUSDc": 1.17079, "AUDJPYc": 96.639, "EURNZDc": 1.95687, "USDCHFc": 0.80455}</t>
+        </is>
+      </c>
+      <c r="E2076" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2077">
+      <c r="A2077" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2077" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:48:36.266551</t>
+        </is>
+      </c>
+      <c r="C2077" t="n">
+        <v>31.37</v>
+      </c>
+      <c r="D2077" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.766, "EURCADc": 1.61098, "AUDCHFc": 0.52662, "EURUSDc": 1.17076}</t>
+        </is>
+      </c>
+      <c r="E2077" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2078">
+      <c r="A2078" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2078" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:48:36.321901</t>
+        </is>
+      </c>
+      <c r="C2078" t="n">
+        <v>-4.37</v>
+      </c>
+      <c r="D2078" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.8637, "EURUSDc": 1.17076, "AUDJPYc": 96.624, "EURNZDc": 1.95706, "USDCHFc": 0.8039}</t>
+        </is>
+      </c>
+      <c r="E2078" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2079">
+      <c r="A2079" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2079" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:48:37.288614</t>
+        </is>
+      </c>
+      <c r="C2079" t="n">
+        <v>31.36</v>
+      </c>
+      <c r="D2079" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.765, "EURCADc": 1.61098, "AUDCHFc": 0.52662, "EURUSDc": 1.17076}</t>
+        </is>
+      </c>
+      <c r="E2079" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2080">
+      <c r="A2080" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2080" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:48:37.334856</t>
+        </is>
+      </c>
+      <c r="C2080" t="n">
+        <v>-4.37</v>
+      </c>
+      <c r="D2080" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.8637, "EURUSDc": 1.17076, "AUDJPYc": 96.624, "EURNZDc": 1.95706, "USDCHFc": 0.8039}</t>
+        </is>
+      </c>
+      <c r="E2080" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2081">
+      <c r="A2081" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2081" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:48:38.302625</t>
+        </is>
+      </c>
+      <c r="C2081" t="n">
+        <v>31.34</v>
+      </c>
+      <c r="D2081" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.765, "EURCADc": 1.61099, "AUDCHFc": 0.52662, "EURUSDc": 1.17077}</t>
+        </is>
+      </c>
+      <c r="E2081" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2082">
+      <c r="A2082" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2082" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:11.585388</t>
+        </is>
+      </c>
+      <c r="C2082" t="n">
+        <v>31.07</v>
+      </c>
+      <c r="D2082" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.798, "EURCADc": 1.61119, "AUDCHFc": 0.52638, "EURUSDc": 1.1708}</t>
+        </is>
+      </c>
+      <c r="E2082" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2083">
+      <c r="A2083" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2083" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:11.603361</t>
+        </is>
+      </c>
+      <c r="C2083" t="n">
+        <v>-5.41</v>
+      </c>
+      <c r="D2083" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86435, "EURUSDc": 1.17082, "AUDJPYc": 96.602, "EURNZDc": 1.95706, "USDCHFc": 0.80361}</t>
+        </is>
+      </c>
+      <c r="E2083" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2084">
+      <c r="A2084" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2084" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:12.605796</t>
+        </is>
+      </c>
+      <c r="C2084" t="n">
+        <v>31.15</v>
+      </c>
+      <c r="D2084" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.797, "EURCADc": 1.61117, "AUDCHFc": 0.52639, "EURUSDc": 1.17077}</t>
+        </is>
+      </c>
+      <c r="E2084" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2085">
+      <c r="A2085" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2085" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:12.626495</t>
+        </is>
+      </c>
+      <c r="C2085" t="n">
+        <v>-5.34</v>
+      </c>
+      <c r="D2085" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86434, "EURUSDc": 1.17077, "AUDJPYc": 96.604, "EURNZDc": 1.95705, "USDCHFc": 0.80362}</t>
+        </is>
+      </c>
+      <c r="E2085" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2086">
+      <c r="A2086" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2086" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:13.629343</t>
+        </is>
+      </c>
+      <c r="C2086" t="n">
+        <v>31.15</v>
+      </c>
+      <c r="D2086" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.796, "EURCADc": 1.61117, "AUDCHFc": 0.52639, "EURUSDc": 1.17076}</t>
+        </is>
+      </c>
+      <c r="E2086" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2087">
+      <c r="A2087" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2087" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:13.644640</t>
+        </is>
+      </c>
+      <c r="C2087" t="n">
+        <v>-5.27</v>
+      </c>
+      <c r="D2087" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86432, "EURUSDc": 1.17076, "AUDJPYc": 96.606, "EURNZDc": 1.95704, "USDCHFc": 0.80363}</t>
+        </is>
+      </c>
+      <c r="E2087" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2088">
+      <c r="A2088" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2088" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:14.654201</t>
+        </is>
+      </c>
+      <c r="C2088" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="D2088" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59838, "GBPJPYc": 199.79, "EURCADc": 1.61112, "AUDCHFc": 0.52641, "EURUSDc": 1.17074}</t>
+        </is>
+      </c>
+      <c r="E2088" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2089">
+      <c r="A2089" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2089" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:14.654201</t>
+        </is>
+      </c>
+      <c r="C2089" t="n">
+        <v>-5.23</v>
+      </c>
+      <c r="D2089" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86432, "EURUSDc": 1.17074, "AUDJPYc": 96.609, "EURNZDc": 1.95704, "USDCHFc": 0.80363}</t>
+        </is>
+      </c>
+      <c r="E2089" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2090">
+      <c r="A2090" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2090" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:15.665520</t>
+        </is>
+      </c>
+      <c r="C2090" t="n">
+        <v>31.19</v>
+      </c>
+      <c r="D2090" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59839, "GBPJPYc": 199.79, "EURCADc": 1.61112, "AUDCHFc": 0.52641, "EURUSDc": 1.17074}</t>
+        </is>
+      </c>
+      <c r="E2090" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2091">
+      <c r="A2091" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2091" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:55:15.681284</t>
+        </is>
+      </c>
+      <c r="C2091" t="n">
+        <v>-5.15</v>
+      </c>
+      <c r="D2091" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86428, "EURUSDc": 1.17074, "AUDJPYc": 96.609, "EURNZDc": 1.95701, "USDCHFc": 0.80365}</t>
+        </is>
+      </c>
+      <c r="E2091" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2092">
+      <c r="A2092" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2092" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:16.895593</t>
+        </is>
+      </c>
+      <c r="C2092" t="n">
+        <v>35.21</v>
+      </c>
+      <c r="D2092" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59732, "GBPJPYc": 199.995, "EURCADc": 1.61226, "AUDCHFc": 0.52646, "EURUSDc": 1.17096}</t>
+        </is>
+      </c>
+      <c r="E2092" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2093">
+      <c r="A2093" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2093" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:17.913589</t>
+        </is>
+      </c>
+      <c r="C2093" t="n">
+        <v>35.24</v>
+      </c>
+      <c r="D2093" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59728, "GBPJPYc": 200.103, "EURCADc": 1.61132, "AUDCHFc": 0.5268, "EURUSDc": 1.17025}</t>
+        </is>
+      </c>
+      <c r="E2093" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2094">
+      <c r="A2094" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2094" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:18.874682</t>
+        </is>
+      </c>
+      <c r="C2094" t="n">
+        <v>-8.35</v>
+      </c>
+      <c r="D2094" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.8686, "EURUSDc": 1.17024, "AUDJPYc": 96.452, "EURNZDc": 1.95978, "USDCHFc": 0.8054}</t>
+        </is>
+      </c>
+      <c r="E2094" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2095">
+      <c r="A2095" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2095" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:18.924399</t>
+        </is>
+      </c>
+      <c r="C2095" t="n">
+        <v>35.31</v>
+      </c>
+      <c r="D2095" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59728, "GBPJPYc": 200.11, "EURCADc": 1.61132, "AUDCHFc": 0.52681, "EURUSDc": 1.17024}</t>
+        </is>
+      </c>
+      <c r="E2095" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2096">
+      <c r="A2096" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2096" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:19.896993</t>
+        </is>
+      </c>
+      <c r="C2096" t="n">
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="D2096" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86859, "EURUSDc": 1.17016, "AUDJPYc": 96.455, "EURNZDc": 1.9597, "USDCHFc": 0.80546}</t>
+        </is>
+      </c>
+      <c r="E2096" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2097">
+      <c r="A2097" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2097" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:19.944532</t>
+        </is>
+      </c>
+      <c r="C2097" t="n">
+        <v>35.49</v>
+      </c>
+      <c r="D2097" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59728, "GBPJPYc": 200.115, "EURCADc": 1.61127, "AUDCHFc": 0.52684, "EURUSDc": 1.17016}</t>
+        </is>
+      </c>
+      <c r="E2097" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2098">
+      <c r="A2098" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2098" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:20.906842</t>
+        </is>
+      </c>
+      <c r="C2098" t="n">
+        <v>-8.109999999999999</v>
+      </c>
+      <c r="D2098" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86857, "EURUSDc": 1.17016, "AUDJPYc": 96.456, "EURNZDc": 1.95972, "USDCHFc": 0.80546}</t>
+        </is>
+      </c>
+      <c r="E2098" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2099">
+      <c r="A2099" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2099" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:20.952567</t>
+        </is>
+      </c>
+      <c r="C2099" t="n">
+        <v>35.56</v>
+      </c>
+      <c r="D2099" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59726, "GBPJPYc": 200.12, "EURCADc": 1.61125, "AUDCHFc": 0.52684, "EURUSDc": 1.17016}</t>
+        </is>
+      </c>
+      <c r="E2099" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2100">
+      <c r="A2100" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2100" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:21.932916</t>
+        </is>
+      </c>
+      <c r="C2100" t="n">
+        <v>-8.130000000000001</v>
+      </c>
+      <c r="D2100" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86857, "EURUSDc": 1.17018, "AUDJPYc": 96.456, "EURNZDc": 1.95972, "USDCHFc": 0.80546}</t>
+        </is>
+      </c>
+      <c r="E2100" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2101">
+      <c r="A2101" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2101" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:21.964477</t>
+        </is>
+      </c>
+      <c r="C2101" t="n">
+        <v>35.53</v>
+      </c>
+      <c r="D2101" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59726, "GBPJPYc": 200.118, "EURCADc": 1.61125, "AUDCHFc": 0.52684, "EURUSDc": 1.17018}</t>
+        </is>
+      </c>
+      <c r="E2101" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2102">
+      <c r="A2102" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2102" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:22.940747</t>
+        </is>
+      </c>
+      <c r="C2102" t="n">
+        <v>-8.08</v>
+      </c>
+      <c r="D2102" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86857, "EURUSDc": 1.17015, "AUDJPYc": 96.458, "EURNZDc": 1.95973, "USDCHFc": 0.80547}</t>
+        </is>
+      </c>
+      <c r="E2102" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2103">
+      <c r="A2103" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2103" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:22.971379</t>
+        </is>
+      </c>
+      <c r="C2103" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="D2103" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59726, "GBPJPYc": 200.123, "EURCADc": 1.61123, "AUDCHFc": 0.52684, "EURUSDc": 1.17015}</t>
+        </is>
+      </c>
+      <c r="E2103" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2104">
+      <c r="A2104" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2104" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:23.953503</t>
+        </is>
+      </c>
+      <c r="C2104" t="n">
+        <v>-8.06</v>
+      </c>
+      <c r="D2104" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86859, "EURUSDc": 1.17014, "AUDJPYc": 96.458, "EURNZDc": 1.95971, "USDCHFc": 0.80548}</t>
+        </is>
+      </c>
+      <c r="E2104" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2105">
+      <c r="A2105" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2105" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:23.984704</t>
+        </is>
+      </c>
+      <c r="C2105" t="n">
+        <v>35.63</v>
+      </c>
+      <c r="D2105" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59725, "GBPJPYc": 200.124, "EURCADc": 1.61123, "AUDCHFc": 0.52684, "EURUSDc": 1.17014}</t>
+        </is>
+      </c>
+      <c r="E2105" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2106">
+      <c r="A2106" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2106" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:24.979733</t>
+        </is>
+      </c>
+      <c r="C2106" t="n">
+        <v>-8.039999999999999</v>
+      </c>
+      <c r="D2106" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86859, "EURUSDc": 1.17013, "AUDJPYc": 96.458, "EURNZDc": 1.95969, "USDCHFc": 0.80547}</t>
+        </is>
+      </c>
+      <c r="E2106" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2107">
+      <c r="A2107" t="n">
+        <v>263006287</v>
+      </c>
+      <c r="B2107" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:25.006118</t>
+        </is>
+      </c>
+      <c r="C2107" t="n">
+        <v>35.66</v>
+      </c>
+      <c r="D2107" t="inlineStr">
+        <is>
+          <t>{"NZDUSDc": 0.59725, "GBPJPYc": 200.124, "EURCADc": 1.61121, "AUDCHFc": 0.52684, "EURUSDc": 1.17013}</t>
+        </is>
+      </c>
+      <c r="E2107" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2108">
+      <c r="A2108" t="n">
+        <v>183459647</v>
+      </c>
+      <c r="B2108" t="inlineStr">
+        <is>
+          <t>2025-08-14T01:15:25.997798</t>
+        </is>
+      </c>
+      <c r="C2108" t="n">
+        <v>-8.050000000000001</v>
+      </c>
+      <c r="D2108" t="inlineStr">
+        <is>
+          <t>{"GBPCADc": 1.86862, "EURUSDc": 1.17013, "AUDJPYc": 96.459, "EURNZDc": 1.95969, "USDCHFc": 0.80547}</t>
+        </is>
+      </c>
+      <c r="E2108" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>